<commit_message>
feat: add file read me
</commit_message>
<xml_diff>
--- a/src/main/webapp/exportExcel/exportQuestion.xlsx
+++ b/src/main/webapp/exportExcel/exportQuestion.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="374">
   <si>
     <t>Nội dung câu hỏi</t>
   </si>
@@ -1071,6 +1071,69 @@
   </si>
   <si>
     <t>5 + 5 = ?</t>
+  </si>
+  <si>
+    <t>1 + 3 = ?</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Toi la ai ?</t>
+  </si>
+  <si>
+    <t>loc</t>
+  </si>
+  <si>
+    <t>huy</t>
+  </si>
+  <si>
+    <t>hung</t>
+  </si>
+  <si>
+    <t>khong co dap dan dung</t>
+  </si>
+  <si>
+    <t>cau hoi 1 ne</t>
+  </si>
+  <si>
+    <t>fsf</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>fsd</t>
+  </si>
+  <si>
+    <t>cau hoi 2</t>
+  </si>
+  <si>
+    <t>fád</t>
+  </si>
+  <si>
+    <t>fsa</t>
+  </si>
+  <si>
+    <t>fsda</t>
+  </si>
+  <si>
+    <t>fsdfsf</t>
+  </si>
+  <si>
+    <t>cau hoi so 78 = ?</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>213</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1180,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -1197,7 +1269,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -3092,6 +3164,219 @@
         <v>216</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>353</v>
+      </c>
+      <c r="B74" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" t="s" s="73">
+        <v>354</v>
+      </c>
+      <c r="F74" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>356</v>
+      </c>
+      <c r="B75" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>83</v>
+      </c>
+      <c r="D75" t="s">
+        <v>39</v>
+      </c>
+      <c r="E75" t="s">
+        <v>357</v>
+      </c>
+      <c r="F75" t="s">
+        <v>358</v>
+      </c>
+      <c r="G75" t="s">
+        <v>359</v>
+      </c>
+      <c r="H75" t="s" s="74">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>361</v>
+      </c>
+      <c r="B76" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" t="s">
+        <v>362</v>
+      </c>
+      <c r="F76" t="s" s="75">
+        <v>363</v>
+      </c>
+      <c r="G76" t="s">
+        <v>364</v>
+      </c>
+      <c r="H76" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>365</v>
+      </c>
+      <c r="B77" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" t="s">
+        <v>366</v>
+      </c>
+      <c r="F77" t="s">
+        <v>367</v>
+      </c>
+      <c r="G77" t="s" s="76">
+        <v>368</v>
+      </c>
+      <c r="H77" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>353</v>
+      </c>
+      <c r="B78" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" t="s" s="77">
+        <v>354</v>
+      </c>
+      <c r="F78" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>356</v>
+      </c>
+      <c r="B79" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" t="s">
+        <v>39</v>
+      </c>
+      <c r="E79" t="s">
+        <v>357</v>
+      </c>
+      <c r="F79" t="s">
+        <v>358</v>
+      </c>
+      <c r="G79" t="s">
+        <v>359</v>
+      </c>
+      <c r="H79" t="s" s="78">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>370</v>
+      </c>
+      <c r="B80" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" t="s" s="79">
+        <v>371</v>
+      </c>
+      <c r="F80" t="s">
+        <v>372</v>
+      </c>
+      <c r="G80" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>353</v>
+      </c>
+      <c r="B81" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" t="s" s="80">
+        <v>354</v>
+      </c>
+      <c r="F81" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>356</v>
+      </c>
+      <c r="B82" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>83</v>
+      </c>
+      <c r="D82" t="s">
+        <v>39</v>
+      </c>
+      <c r="E82" t="s">
+        <v>357</v>
+      </c>
+      <c r="F82" t="s">
+        <v>358</v>
+      </c>
+      <c r="G82" t="s">
+        <v>359</v>
+      </c>
+      <c r="H82" t="s" s="81">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>